<commit_message>
quick analysis of data using formulas
</commit_message>
<xml_diff>
--- a/blank-data-file.xlsx
+++ b/blank-data-file.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="219">
   <si>
     <t>Name</t>
   </si>
@@ -678,14 +678,48 @@
   </si>
   <si>
     <t>NZ</t>
+  </si>
+  <si>
+    <t>Count of Employees</t>
+  </si>
+  <si>
+    <t>Average Salary</t>
+  </si>
+  <si>
+    <t>Average Age</t>
+  </si>
+  <si>
+    <t>Average Tenure</t>
+  </si>
+  <si>
+    <t>Female Ratio %</t>
+  </si>
+  <si>
+    <t>Tenure</t>
+  </si>
+  <si>
+    <t>Female Count</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of employees &gt; </t>
+  </si>
+  <si>
+    <t>oyees salary &gt; 90,000</t>
+  </si>
+  <si>
+    <t>&gt; $90,000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -734,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -742,37 +776,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -785,13 +808,40 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -808,8 +858,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="9">
-    <queryTableFields count="8">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="11" unboundColumnsRight="1">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Name" tableColumnId="25"/>
       <queryTableField id="2" name="Gender" tableColumnId="26"/>
       <queryTableField id="3" name="Age" tableColumnId="27"/>
@@ -818,6 +868,7 @@
       <queryTableField id="6" name="Department" tableColumnId="30"/>
       <queryTableField id="7" name="Salary" tableColumnId="31"/>
       <queryTableField id="8" name="Country" tableColumnId="32"/>
+      <queryTableField id="10" dataBound="0" tableColumnId="1"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -832,7 +883,7 @@
     <tableColumn id="3" name="Department"/>
     <tableColumn id="4" name="Age" totalsRowFunction="average"/>
     <tableColumn id="5" name="Date Joined"/>
-    <tableColumn id="6" name="Salary" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="6" name="Salary" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="7" name="Rating" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -840,17 +891,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Staff" displayName="Staff" ref="A1:H184" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H184"/>
-  <tableColumns count="8">
-    <tableColumn id="25" uniqueName="25" name="Name" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="26" uniqueName="26" name="Gender" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="27" uniqueName="27" name="Age" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="28" uniqueName="28" name="Rating" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="29" uniqueName="29" name="Date Joined" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="30" uniqueName="30" name="Department" queryTableFieldId="6" dataDxfId="2"/>
-    <tableColumn id="31" uniqueName="31" name="Salary" queryTableFieldId="7" dataDxfId="1"/>
-    <tableColumn id="32" uniqueName="32" name="Country" queryTableFieldId="8" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Staff" displayName="Staff" ref="A1:I184" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I184"/>
+  <tableColumns count="9">
+    <tableColumn id="25" uniqueName="25" name="Name" queryTableFieldId="1" dataDxfId="11"/>
+    <tableColumn id="26" uniqueName="26" name="Gender" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="27" uniqueName="27" name="Age" queryTableFieldId="3" dataDxfId="9"/>
+    <tableColumn id="28" uniqueName="28" name="Rating" queryTableFieldId="4" dataDxfId="6"/>
+    <tableColumn id="29" uniqueName="29" name="Date Joined" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="30" uniqueName="30" name="Department" queryTableFieldId="6" dataDxfId="5"/>
+    <tableColumn id="31" uniqueName="31" name="Salary" queryTableFieldId="7" dataDxfId="8"/>
+    <tableColumn id="32" uniqueName="32" name="Country" queryTableFieldId="8" dataDxfId="3"/>
+    <tableColumn id="1" uniqueName="1" name="Tenure" queryTableFieldId="10" dataDxfId="2">
+      <calculatedColumnFormula>(TODAY()-Staff[[#This Row],[Date Joined]])/365</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -864,7 +918,7 @@
     <tableColumn id="2" name="Gender"/>
     <tableColumn id="3" name="Age"/>
     <tableColumn id="4" name="Rating"/>
-    <tableColumn id="5" name="Date Joined" dataDxfId="11"/>
+    <tableColumn id="5" name="Date Joined" dataDxfId="7"/>
     <tableColumn id="6" name="Department"/>
     <tableColumn id="7" name="Salary"/>
   </tableColumns>
@@ -1171,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -3521,7 +3575,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:C105">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3535,10 +3589,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:H184"/>
+  <dimension ref="A1:N184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,13 +3601,16 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3566,7 +3623,7 @@
       <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -3578,8 +3635,11 @@
       <c r="H1" s="6" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>156</v>
       </c>
@@ -3598,14 +3658,21 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>112650</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6712328767123288</v>
+      </c>
+      <c r="N2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>176</v>
       </c>
@@ -3624,14 +3691,25 @@
       <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>43840</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2027397260273971</v>
+      </c>
+      <c r="K3" t="s">
+        <v>208</v>
+      </c>
+      <c r="M3">
+        <f>COUNTA(Staff[Name])</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>143</v>
       </c>
@@ -3650,14 +3728,29 @@
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>103550</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.189041095890411</v>
+      </c>
+      <c r="K4" t="s">
+        <v>209</v>
+      </c>
+      <c r="M4" s="5">
+        <f>AVERAGE(G:G)</f>
+        <v>77173.715846994543</v>
+      </c>
+      <c r="N4">
+        <f>MEDIAN(Staff[Salary])</f>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>201</v>
       </c>
@@ -3676,14 +3769,29 @@
       <c r="F5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>45510</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.0767123287671234</v>
+      </c>
+      <c r="K5" t="s">
+        <v>210</v>
+      </c>
+      <c r="M5">
+        <f>AVERAGE(C:C)</f>
+        <v>30.42622950819672</v>
+      </c>
+      <c r="N5">
+        <f>MEDIAN(Staff[Age])</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>142</v>
       </c>
@@ -3702,14 +3810,29 @@
       <c r="F6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>115440</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.7726027397260276</v>
+      </c>
+      <c r="K6" t="s">
+        <v>211</v>
+      </c>
+      <c r="M6">
+        <f ca="1">AVERAGE(Staff[Tenure])</f>
+        <v>1.8190882551089151</v>
+      </c>
+      <c r="N6">
+        <f ca="1">MEDIAN(Staff[Tenure])</f>
+        <v>1.8410958904109589</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>202</v>
       </c>
@@ -3728,14 +3851,25 @@
       <c r="F7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>56870</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2712328767123289</v>
+      </c>
+      <c r="K7" t="s">
+        <v>212</v>
+      </c>
+      <c r="M7" s="10">
+        <f>85/183</f>
+        <v>0.46448087431693991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>169</v>
       </c>
@@ -3754,14 +3888,25 @@
       <c r="F8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>92700</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6109589041095891</v>
+      </c>
+      <c r="K8" t="s">
+        <v>214</v>
+      </c>
+      <c r="M8">
+        <f>COUNTIFS(Staff[Gender],"Female")</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>145</v>
       </c>
@@ -3780,14 +3925,18 @@
       <c r="F9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>91310</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0520547945205478</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>115</v>
       </c>
@@ -3806,14 +3955,31 @@
       <c r="F10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>74550</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.117808219178082</v>
+      </c>
+      <c r="K10" t="s">
+        <v>216</v>
+      </c>
+      <c r="L10" t="s">
+        <v>217</v>
+      </c>
+      <c r="M10" t="s">
+        <v>218</v>
+      </c>
+      <c r="N10" s="10">
+        <f>173/183</f>
+        <v>0.94535519125683065</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>128</v>
       </c>
@@ -3832,14 +3998,18 @@
       <c r="F11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>109190</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1835616438356165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>194</v>
       </c>
@@ -3858,14 +4028,18 @@
       <c r="F12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>104410</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.128767123287671</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>177</v>
       </c>
@@ -3884,14 +4058,18 @@
       <c r="F13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>96800</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.515068493150685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>123</v>
       </c>
@@ -3910,14 +4088,18 @@
       <c r="F14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>48170</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>3.0602739726027397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>140</v>
       </c>
@@ -3936,14 +4118,18 @@
       <c r="F15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>37920</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.8904109589041096</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>178</v>
       </c>
@@ -3962,14 +4148,18 @@
       <c r="F16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>112650</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.2465753424657535</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>165</v>
       </c>
@@ -3988,14 +4178,18 @@
       <c r="F17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>49630</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1972602739726028</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>199</v>
       </c>
@@ -4014,14 +4208,18 @@
       <c r="F18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>118840</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>3.1205479452054794</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>159</v>
       </c>
@@ -4040,14 +4238,18 @@
       <c r="F19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>69710</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.84383561643835614</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>197</v>
       </c>
@@ -4066,14 +4268,18 @@
       <c r="F20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>79570</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1342465753424658</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>154</v>
       </c>
@@ -4092,14 +4298,18 @@
       <c r="F21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>76900</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9424657534246574</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>182</v>
       </c>
@@ -4118,14 +4328,18 @@
       <c r="F22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>54970</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.8054794520547945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>118</v>
       </c>
@@ -4144,14 +4358,18 @@
       <c r="F23" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <v>88050</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2465753424657535</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>192</v>
       </c>
@@ -4170,14 +4388,18 @@
       <c r="F24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>36040</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.4767123287671233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>111</v>
       </c>
@@ -4196,14 +4418,18 @@
       <c r="F25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>75000</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0383561643835617</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>149</v>
       </c>
@@ -4222,14 +4448,18 @@
       <c r="F26" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="5">
         <v>40400</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1808219178082191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>196</v>
       </c>
@@ -4248,14 +4478,18 @@
       <c r="F27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>100420</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.2931506849315069</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>120</v>
       </c>
@@ -4274,14 +4508,18 @@
       <c r="F28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="5">
         <v>58100</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3506849315068492</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>114</v>
       </c>
@@ -4300,14 +4538,18 @@
       <c r="F29" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>114870</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.30684931506849317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>158</v>
       </c>
@@ -4326,14 +4568,18 @@
       <c r="F30" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <v>41570</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.5013698630136987</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>173</v>
       </c>
@@ -4352,14 +4598,18 @@
       <c r="F31" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <v>112570</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.81369863013698629</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>151</v>
       </c>
@@ -4378,14 +4628,18 @@
       <c r="F32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="5">
         <v>47360</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.5561643835616437</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>126</v>
       </c>
@@ -4404,14 +4658,18 @@
       <c r="F33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="5">
         <v>65920</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.3041095890410959</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>200</v>
       </c>
@@ -4430,14 +4688,18 @@
       <c r="F34" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <v>99970</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.441095890410959</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>133</v>
       </c>
@@ -4456,14 +4718,18 @@
       <c r="F35" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="5">
         <v>80700</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.2712328767123289</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>155</v>
       </c>
@@ -4482,14 +4748,18 @@
       <c r="F36" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="5">
         <v>52610</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.978082191780822</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>180</v>
       </c>
@@ -4508,14 +4778,18 @@
       <c r="F37" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="5">
         <v>112110</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6794520547945204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>152</v>
       </c>
@@ -4534,14 +4808,18 @@
       <c r="F38" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="5">
         <v>119110</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.8383561643835615</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>150</v>
       </c>
@@ -4560,14 +4838,18 @@
       <c r="F39" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="5">
         <v>112780</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9534246575342467</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>175</v>
       </c>
@@ -4586,14 +4868,18 @@
       <c r="F40" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="5">
         <v>114890</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.9424657534246577</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>146</v>
       </c>
@@ -4612,14 +4898,18 @@
       <c r="F41" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="5">
         <v>48980</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.6191780821917807</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>170</v>
       </c>
@@ -4638,14 +4928,18 @@
       <c r="F42" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42" s="5">
         <v>75880</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.5123287671232877</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>167</v>
       </c>
@@ -4664,14 +4958,18 @@
       <c r="F43" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>53240</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.1945205479452055</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>122</v>
       </c>
@@ -4690,14 +4988,18 @@
       <c r="F44" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="5">
         <v>85000</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9178082191780821</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>179</v>
       </c>
@@ -4716,14 +5018,18 @@
       <c r="F45" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="5">
         <v>33920</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3095890410958904</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>188</v>
       </c>
@@ -4742,14 +5048,18 @@
       <c r="F46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="6">
+      <c r="G46" s="5">
         <v>75280</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.3123287671232875</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>130</v>
       </c>
@@ -4768,14 +5078,18 @@
       <c r="F47" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47" s="5">
         <v>58940</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3780821917808219</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>136</v>
       </c>
@@ -4794,14 +5108,18 @@
       <c r="F48" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48" s="5">
         <v>104770</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.8410958904109589</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>125</v>
       </c>
@@ -4820,14 +5138,18 @@
       <c r="F49" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49" s="5">
         <v>57090</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0849315068493151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>160</v>
       </c>
@@ -4846,14 +5168,18 @@
       <c r="F50" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G50" s="5">
         <v>91650</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.5287671232876714</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>183</v>
       </c>
@@ -4872,14 +5198,18 @@
       <c r="F51" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="5">
         <v>70270</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1698630136986301</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>129</v>
       </c>
@@ -4898,14 +5228,18 @@
       <c r="F52" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52" s="5">
         <v>75970</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6657534246575341</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>112</v>
       </c>
@@ -4924,14 +5258,18 @@
       <c r="F53" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53" s="5">
         <v>90700</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.4246575342465753</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>131</v>
       </c>
@@ -4950,14 +5288,18 @@
       <c r="F54" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="5">
         <v>60570</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3424657534246576</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>134</v>
       </c>
@@ -4976,14 +5318,18 @@
       <c r="F55" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55" s="5">
         <v>115920</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.7232876712328768</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>186</v>
       </c>
@@ -5002,14 +5348,18 @@
       <c r="F56" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G56" s="6">
+      <c r="G56" s="5">
         <v>65360</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.989041095890411</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>116</v>
       </c>
@@ -5028,14 +5378,18 @@
       <c r="F57" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G57" s="6">
+      <c r="G57" s="5">
         <v>64000</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.5397260273972602</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>195</v>
       </c>
@@ -5054,14 +5408,18 @@
       <c r="F58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G58" s="6">
+      <c r="G58" s="5">
         <v>92450</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9561643835616438</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>113</v>
       </c>
@@ -5080,14 +5438,18 @@
       <c r="F59" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G59" s="6">
+      <c r="G59" s="5">
         <v>48950</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7726027397260273</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>185</v>
       </c>
@@ -5106,14 +5468,18 @@
       <c r="F60" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G60" s="5">
         <v>83750</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.2931506849315069</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>166</v>
       </c>
@@ -5132,14 +5498,18 @@
       <c r="F61" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G61" s="6">
+      <c r="G61" s="5">
         <v>87620</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2493150684931509</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>184</v>
       </c>
@@ -5158,14 +5528,18 @@
       <c r="F62" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G62" s="6">
+      <c r="G62" s="5">
         <v>68900</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7013698630136986</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>157</v>
       </c>
@@ -5184,14 +5558,18 @@
       <c r="F63" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G63" s="6">
+      <c r="G63" s="5">
         <v>53540</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9013698630136986</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>172</v>
       </c>
@@ -5210,14 +5588,18 @@
       <c r="F64" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G64" s="6">
+      <c r="G64" s="5">
         <v>43510</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.92876712328767119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>127</v>
       </c>
@@ -5236,14 +5618,18 @@
       <c r="F65" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G65" s="6">
+      <c r="G65" s="5">
         <v>109160</v>
       </c>
       <c r="H65" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.1397260273972605</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>198</v>
       </c>
@@ -5262,14 +5648,18 @@
       <c r="F66" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G66" s="6">
+      <c r="G66" s="5">
         <v>99750</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.4465753424657533</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>124</v>
       </c>
@@ -5288,14 +5678,18 @@
       <c r="F67" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G67" s="6">
+      <c r="G67" s="5">
         <v>41980</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.7753424657534245</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>187</v>
       </c>
@@ -5314,14 +5708,18 @@
       <c r="F68" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G68" s="6">
+      <c r="G68" s="5">
         <v>71380</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2602739726027399</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>191</v>
       </c>
@@ -5340,14 +5738,18 @@
       <c r="F69" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G69" s="6">
+      <c r="G69" s="5">
         <v>113280</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.5068493150684932</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>181</v>
       </c>
@@ -5366,14 +5768,18 @@
       <c r="F70" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G70" s="6">
+      <c r="G70" s="5">
         <v>86570</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.95890410958904104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>139</v>
       </c>
@@ -5392,14 +5798,18 @@
       <c r="F71" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G71" s="6">
+      <c r="G71" s="5">
         <v>53540</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.0465753424657533</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>190</v>
       </c>
@@ -5418,14 +5828,18 @@
       <c r="F72" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G72" s="6">
+      <c r="G72" s="5">
         <v>69070</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.252054794520548</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>121</v>
       </c>
@@ -5444,14 +5858,18 @@
       <c r="F73" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G73" s="6">
+      <c r="G73" s="5">
         <v>67910</v>
       </c>
       <c r="H73" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.106849315068493</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>119</v>
       </c>
@@ -5470,14 +5888,18 @@
       <c r="F74" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G74" s="6">
+      <c r="G74" s="5">
         <v>69120</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.419178082191781</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>132</v>
       </c>
@@ -5496,14 +5918,18 @@
       <c r="F75" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G75" s="6">
+      <c r="G75" s="5">
         <v>60130</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.4986301369863013</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>161</v>
       </c>
@@ -5522,14 +5948,18 @@
       <c r="F76" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G76" s="6">
+      <c r="G76" s="5">
         <v>106460</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9698630136986301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>148</v>
       </c>
@@ -5548,14 +5978,18 @@
       <c r="F77" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G77" s="6">
+      <c r="G77" s="5">
         <v>118100</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9397260273972603</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>164</v>
       </c>
@@ -5574,14 +6008,18 @@
       <c r="F78" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G78" s="6">
+      <c r="G78" s="5">
         <v>78390</v>
       </c>
       <c r="H78" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7232876712328766</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>147</v>
       </c>
@@ -5600,14 +6038,18 @@
       <c r="F79" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G79" s="6">
+      <c r="G79" s="5">
         <v>114180</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.84383561643835614</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>189</v>
       </c>
@@ -5626,14 +6068,18 @@
       <c r="F80" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G80" s="5">
         <v>104120</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3890410958904109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>138</v>
       </c>
@@ -5652,14 +6098,18 @@
       <c r="F81" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G81" s="6">
+      <c r="G81" s="5">
         <v>67950</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.252054794520548</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>137</v>
       </c>
@@ -5678,14 +6128,18 @@
       <c r="F82" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G82" s="6">
+      <c r="G82" s="5">
         <v>34980</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>3.1095890410958904</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>153</v>
       </c>
@@ -5704,14 +6158,18 @@
       <c r="F83" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G83" s="6">
+      <c r="G83" s="5">
         <v>62780</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.7671232876712328</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>117</v>
       </c>
@@ -5730,14 +6188,18 @@
       <c r="F84" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G84" s="6">
+      <c r="G84" s="5">
         <v>107700</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9178082191780821</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>168</v>
       </c>
@@ -5756,14 +6218,18 @@
       <c r="F85" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G85" s="6">
+      <c r="G85" s="5">
         <v>65700</v>
       </c>
       <c r="H85" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.1232876712328768</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>135</v>
       </c>
@@ -5782,14 +6248,18 @@
       <c r="F86" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G86" s="6">
+      <c r="G86" s="5">
         <v>75480</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.1479452054794521</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>174</v>
       </c>
@@ -5808,14 +6278,18 @@
       <c r="F87" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G87" s="6">
+      <c r="G87" s="5">
         <v>53870</v>
       </c>
       <c r="H87" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7780821917808218</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>141</v>
       </c>
@@ -5834,14 +6308,18 @@
       <c r="F88" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G88" s="6">
+      <c r="G88" s="5">
         <v>78540</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.8191780821917809</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>193</v>
       </c>
@@ -5860,14 +6338,18 @@
       <c r="F89" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G89" s="6">
+      <c r="G89" s="5">
         <v>58960</v>
       </c>
       <c r="H89" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.408219178082192</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>162</v>
       </c>
@@ -5886,14 +6368,18 @@
       <c r="F90" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G90" s="5">
         <v>70610</v>
       </c>
       <c r="H90" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.095890410958904</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>171</v>
       </c>
@@ -5912,14 +6398,18 @@
       <c r="F91" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G91" s="6">
+      <c r="G91" s="5">
         <v>59430</v>
       </c>
       <c r="H91" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.5095890410958903</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>144</v>
       </c>
@@ -5938,14 +6428,18 @@
       <c r="F92" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G92" s="6">
+      <c r="G92" s="5">
         <v>48530</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.252054794520548</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>163</v>
       </c>
@@ -5964,14 +6458,18 @@
       <c r="F93" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G93" s="6">
+      <c r="G93" s="5">
         <v>96140</v>
       </c>
       <c r="H93" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6520547945205482</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>58</v>
       </c>
@@ -5990,14 +6488,18 @@
       <c r="F94" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G94" s="6">
+      <c r="G94" s="5">
         <v>112780</v>
       </c>
       <c r="H94" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7835616438356163</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>70</v>
       </c>
@@ -6016,14 +6518,18 @@
       <c r="F95" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G95" s="6">
+      <c r="G95" s="5">
         <v>70610</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.92876712328767119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>75</v>
       </c>
@@ -6042,14 +6548,18 @@
       <c r="F96" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G96" s="6">
+      <c r="G96" s="5">
         <v>53240</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.0273972602739727</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>49</v>
       </c>
@@ -6068,14 +6578,18 @@
       <c r="F97" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G97" s="6">
+      <c r="G97" s="5">
         <v>115440</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6054794520547944</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>65</v>
       </c>
@@ -6094,14 +6608,18 @@
       <c r="F98" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G98" s="6">
+      <c r="G98" s="5">
         <v>53540</v>
       </c>
       <c r="H98" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7315068493150685</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>81</v>
       </c>
@@ -6120,14 +6638,18 @@
       <c r="F99" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G99" s="6">
+      <c r="G99" s="5">
         <v>112570</v>
       </c>
       <c r="H99" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.64657534246575343</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>51</v>
       </c>
@@ -6146,14 +6668,18 @@
       <c r="F100" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G100" s="6">
+      <c r="G100" s="5">
         <v>48530</v>
       </c>
       <c r="H100" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0849315068493151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>61</v>
       </c>
@@ -6172,14 +6698,18 @@
       <c r="F101" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G101" s="6">
+      <c r="G101" s="5">
         <v>62780</v>
       </c>
       <c r="H101" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>82</v>
       </c>
@@ -6198,14 +6728,18 @@
       <c r="F102" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G102" s="6">
+      <c r="G102" s="5">
         <v>53870</v>
       </c>
       <c r="H102" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.6109589041095891</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>60</v>
       </c>
@@ -6224,14 +6758,18 @@
       <c r="F103" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G103" s="6">
+      <c r="G103" s="5">
         <v>119110</v>
       </c>
       <c r="H103" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6712328767123288</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>87</v>
       </c>
@@ -6250,14 +6788,18 @@
       <c r="F104" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G104" s="6">
+      <c r="G104" s="5">
         <v>112110</v>
       </c>
       <c r="H104" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.5123287671232877</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>76</v>
       </c>
@@ -6276,14 +6818,18 @@
       <c r="F105" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G105" s="6">
+      <c r="G105" s="5">
         <v>65700</v>
       </c>
       <c r="H105" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9561643835616438</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>97</v>
       </c>
@@ -6302,14 +6848,18 @@
       <c r="F106" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G106" s="6">
+      <c r="G106" s="5">
         <v>69070</v>
       </c>
       <c r="H106" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0849315068493151</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>22</v>
       </c>
@@ -6328,14 +6878,18 @@
       <c r="F107" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G107" s="6">
+      <c r="G107" s="5">
         <v>107700</v>
       </c>
       <c r="H107" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.747945205479452</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>84</v>
       </c>
@@ -6354,14 +6908,18 @@
       <c r="F108" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G108" s="6">
+      <c r="G108" s="5">
         <v>43840</v>
       </c>
       <c r="H108" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.0356164383561643</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>105</v>
       </c>
@@ -6380,14 +6938,18 @@
       <c r="F109" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G109" s="6">
+      <c r="G109" s="5">
         <v>99750</v>
       </c>
       <c r="H109" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2849315068493152</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>47</v>
       </c>
@@ -6406,14 +6968,18 @@
       <c r="F110" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G110" s="6">
+      <c r="G110" s="5">
         <v>37920</v>
       </c>
       <c r="H110" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.7205479452054795</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>31</v>
       </c>
@@ -6432,14 +6998,18 @@
       <c r="F111" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G111" s="6">
+      <c r="G111" s="5">
         <v>57090</v>
       </c>
       <c r="H111" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.9178082191780822</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>30</v>
       </c>
@@ -6458,14 +7028,18 @@
       <c r="F112" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G112" s="6">
+      <c r="G112" s="5">
         <v>41980</v>
       </c>
       <c r="H112" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6082191780821917</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="6" t="s">
         <v>78</v>
       </c>
@@ -6484,14 +7058,18 @@
       <c r="F113" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G113" s="6">
+      <c r="G113" s="5">
         <v>75880</v>
       </c>
       <c r="H113" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.3424657534246576</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>36</v>
       </c>
@@ -6510,14 +7088,18 @@
       <c r="F114" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G114" s="6">
+      <c r="G114" s="5">
         <v>58940</v>
       </c>
       <c r="H114" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.2164383561643837</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
         <v>27</v>
       </c>
@@ -6536,14 +7118,18 @@
       <c r="F115" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G115" s="6">
+      <c r="G115" s="5">
         <v>67910</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9397260273972603</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>26</v>
       </c>
@@ -6562,14 +7148,18 @@
       <c r="F116" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G116" s="6">
+      <c r="G116" s="5">
         <v>58100</v>
       </c>
       <c r="H116" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.189041095890411</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
         <v>53</v>
       </c>
@@ -6588,14 +7178,18 @@
       <c r="F117" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G117" s="6">
+      <c r="G117" s="5">
         <v>48980</v>
       </c>
       <c r="H117" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.452054794520548</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>20</v>
       </c>
@@ -6614,14 +7208,18 @@
       <c r="F118" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G118" s="6">
+      <c r="G118" s="5">
         <v>64000</v>
       </c>
       <c r="H118" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3698630136986301</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
         <v>7</v>
       </c>
@@ -6640,14 +7238,18 @@
       <c r="F119" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G119" s="6">
+      <c r="G119" s="5">
         <v>75000</v>
       </c>
       <c r="H119" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.87123287671232874</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>74</v>
       </c>
@@ -6666,14 +7268,18 @@
       <c r="F120" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G120" s="6">
+      <c r="G120" s="5">
         <v>87620</v>
       </c>
       <c r="H120" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.0821917808219177</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>44</v>
       </c>
@@ -6692,14 +7298,18 @@
       <c r="F121" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G121" s="6">
+      <c r="G121" s="5">
         <v>34980</v>
       </c>
       <c r="H121" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.9424657534246577</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>35</v>
       </c>
@@ -6718,14 +7328,18 @@
       <c r="F122" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G122" s="6">
+      <c r="G122" s="5">
         <v>75970</v>
       </c>
       <c r="H122" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.4986301369863013</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>38</v>
       </c>
@@ -6744,14 +7358,18 @@
       <c r="F123" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G123" s="6">
+      <c r="G123" s="5">
         <v>60130</v>
       </c>
       <c r="H123" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3287671232876712</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>41</v>
       </c>
@@ -6770,14 +7388,18 @@
       <c r="F124" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G124" s="6">
+      <c r="G124" s="5">
         <v>75480</v>
       </c>
       <c r="H124" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9808219178082191</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>40</v>
       </c>
@@ -6796,14 +7418,18 @@
       <c r="F125" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G125" s="6">
+      <c r="G125" s="5">
         <v>115920</v>
       </c>
       <c r="H125" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.5561643835616437</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>48</v>
       </c>
@@ -6822,14 +7448,18 @@
       <c r="F126" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G126" s="6">
+      <c r="G126" s="5">
         <v>78540</v>
       </c>
       <c r="H126" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.6520547945205479</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>34</v>
       </c>
@@ -6848,14 +7478,18 @@
       <c r="F127" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G127" s="6">
+      <c r="G127" s="5">
         <v>109190</v>
       </c>
       <c r="H127" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0164383561643835</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>73</v>
       </c>
@@ -6874,14 +7508,18 @@
       <c r="F128" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G128" s="6">
+      <c r="G128" s="5">
         <v>49630</v>
       </c>
       <c r="H128" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0301369863013699</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>107</v>
       </c>
@@ -6900,14 +7538,18 @@
       <c r="F129" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G129" s="6">
+      <c r="G129" s="5">
         <v>99970</v>
       </c>
       <c r="H129" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.2794520547945205</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>71</v>
       </c>
@@ -6926,14 +7568,18 @@
       <c r="F130" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G130" s="6">
+      <c r="G130" s="5">
         <v>96140</v>
       </c>
       <c r="H130" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.484931506849315</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>50</v>
       </c>
@@ -6952,14 +7598,18 @@
       <c r="F131" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G131" s="6">
+      <c r="G131" s="5">
         <v>103550</v>
       </c>
       <c r="H131" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.021917808219178</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>14</v>
       </c>
@@ -6978,14 +7628,18 @@
       <c r="F132" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G132" s="6">
+      <c r="G132" s="5">
         <v>48950</v>
       </c>
       <c r="H132" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.6054794520547946</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>63</v>
       </c>
@@ -7004,14 +7658,18 @@
       <c r="F133" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G133" s="6">
+      <c r="G133" s="5">
         <v>52610</v>
       </c>
       <c r="H133" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.810958904109589</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>72</v>
       </c>
@@ -7030,14 +7688,18 @@
       <c r="F134" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G134" s="6">
+      <c r="G134" s="5">
         <v>78390</v>
       </c>
       <c r="H134" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.5561643835616439</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>88</v>
       </c>
@@ -7056,14 +7718,18 @@
       <c r="F135" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G135" s="6">
+      <c r="G135" s="5">
         <v>86570</v>
       </c>
       <c r="H135" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.78904109589041094</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>92</v>
       </c>
@@ -7082,14 +7748,18 @@
       <c r="F136" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G136" s="6">
+      <c r="G136" s="5">
         <v>83750</v>
       </c>
       <c r="H136" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1260273972602739</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
         <v>102</v>
       </c>
@@ -7108,14 +7778,18 @@
       <c r="F137" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G137" s="6">
+      <c r="G137" s="5">
         <v>92450</v>
       </c>
       <c r="H137" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7863013698630137</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>64</v>
       </c>
@@ -7134,14 +7808,18 @@
       <c r="F138" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G138" s="6">
+      <c r="G138" s="5">
         <v>112650</v>
       </c>
       <c r="H138" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.504109589041096</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
         <v>104</v>
       </c>
@@ -7160,14 +7838,18 @@
       <c r="F139" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G139" s="6">
+      <c r="G139" s="5">
         <v>79570</v>
       </c>
       <c r="H139" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.9671232876712329</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>91</v>
       </c>
@@ -7186,14 +7868,18 @@
       <c r="F140" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G140" s="6">
+      <c r="G140" s="5">
         <v>68900</v>
       </c>
       <c r="H140" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.5342465753424657</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
         <v>39</v>
       </c>
@@ -7212,14 +7898,18 @@
       <c r="F141" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G141" s="6">
+      <c r="G141" s="5">
         <v>80700</v>
       </c>
       <c r="H141" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1041095890410959</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>100</v>
       </c>
@@ -7238,14 +7928,18 @@
       <c r="F142" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G142" s="6">
+      <c r="G142" s="5">
         <v>58960</v>
       </c>
       <c r="H142" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2465753424657535</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
         <v>106</v>
       </c>
@@ -7264,14 +7958,18 @@
       <c r="F143" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G143" s="6">
+      <c r="G143" s="5">
         <v>118840</v>
       </c>
       <c r="H143" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.9534246575342467</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>29</v>
       </c>
@@ -7290,14 +7988,18 @@
       <c r="F144" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G144" s="6">
+      <c r="G144" s="5">
         <v>48170</v>
       </c>
       <c r="H144" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.893150684931507</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
         <v>108</v>
       </c>
@@ -7316,14 +8018,18 @@
       <c r="F145" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G145" s="6">
+      <c r="G145" s="5">
         <v>45510</v>
       </c>
       <c r="H145" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9095890410958904</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>83</v>
       </c>
@@ -7342,14 +8048,18 @@
       <c r="F146" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G146" s="6">
+      <c r="G146" s="5">
         <v>114890</v>
       </c>
       <c r="H146" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.7726027397260276</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
         <v>67</v>
       </c>
@@ -7368,14 +8078,18 @@
       <c r="F147" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G147" s="6">
+      <c r="G147" s="5">
         <v>69710</v>
       </c>
       <c r="H147" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.67671232876712328</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>94</v>
       </c>
@@ -7394,14 +8108,18 @@
       <c r="F148" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G148" s="6">
+      <c r="G148" s="5">
         <v>71380</v>
       </c>
       <c r="H148" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.0931506849315067</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
         <v>33</v>
       </c>
@@ -7420,14 +8138,18 @@
       <c r="F149" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G149" s="6">
+      <c r="G149" s="5">
         <v>109160</v>
       </c>
       <c r="H149" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9726027397260273</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>98</v>
       </c>
@@ -7446,14 +8168,18 @@
       <c r="F150" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G150" s="6">
+      <c r="G150" s="5">
         <v>113280</v>
       </c>
       <c r="H150" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3369863013698631</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>25</v>
       </c>
@@ -7472,14 +8198,18 @@
       <c r="F151" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G151" s="6">
+      <c r="G151" s="5">
         <v>69120</v>
       </c>
       <c r="H151" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2575342465753425</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>55</v>
       </c>
@@ -7498,14 +8228,18 @@
       <c r="F152" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G152" s="6">
+      <c r="G152" s="5">
         <v>118100</v>
       </c>
       <c r="H152" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7698630136986302</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
         <v>62</v>
       </c>
@@ -7524,14 +8258,18 @@
       <c r="F153" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G153" s="6">
+      <c r="G153" s="5">
         <v>76900</v>
       </c>
       <c r="H153" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.7726027397260273</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>17</v>
       </c>
@@ -7550,14 +8288,18 @@
       <c r="F154" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G154" s="6">
+      <c r="G154" s="5">
         <v>114870</v>
       </c>
       <c r="H154" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.14246575342465753</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>52</v>
       </c>
@@ -7576,14 +8318,18 @@
       <c r="F155" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G155" s="6">
+      <c r="G155" s="5">
         <v>91310</v>
       </c>
       <c r="H155" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.8849315068493151</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>43</v>
       </c>
@@ -7602,14 +8348,18 @@
       <c r="F156" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G156" s="6">
+      <c r="G156" s="5">
         <v>104770</v>
       </c>
       <c r="H156" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.6739726027397259</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
         <v>89</v>
       </c>
@@ -7628,14 +8378,18 @@
       <c r="F157" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G157" s="6">
+      <c r="G157" s="5">
         <v>54970</v>
       </c>
       <c r="H157" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.6383561643835618</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>11</v>
       </c>
@@ -7654,14 +8408,18 @@
       <c r="F158" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G158" s="6">
+      <c r="G158" s="5">
         <v>90700</v>
       </c>
       <c r="H158" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I158" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.2630136986301368</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
         <v>109</v>
       </c>
@@ -7680,14 +8438,18 @@
       <c r="F159" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G159" s="6">
+      <c r="G159" s="5">
         <v>56870</v>
       </c>
       <c r="H159" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.1041095890410957</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>77</v>
       </c>
@@ -7706,14 +8468,18 @@
       <c r="F160" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G160" s="6">
+      <c r="G160" s="5">
         <v>92700</v>
       </c>
       <c r="H160" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I160" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.4438356164383563</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>32</v>
       </c>
@@ -7732,14 +8498,18 @@
       <c r="F161" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G161" s="6">
+      <c r="G161" s="5">
         <v>65920</v>
       </c>
       <c r="H161" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.1369863013698631</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
         <v>59</v>
       </c>
@@ -7758,14 +8528,18 @@
       <c r="F162" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G162" s="6">
+      <c r="G162" s="5">
         <v>47360</v>
       </c>
       <c r="H162" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.3890410958904109</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
         <v>37</v>
       </c>
@@ -7784,14 +8558,18 @@
       <c r="F163" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G163" s="6">
+      <c r="G163" s="5">
         <v>60570</v>
       </c>
       <c r="H163" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1808219178082191</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>96</v>
       </c>
@@ -7810,14 +8588,18 @@
       <c r="F164" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G164" s="6">
+      <c r="G164" s="5">
         <v>104120</v>
       </c>
       <c r="H164" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.2273972602739727</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
         <v>23</v>
       </c>
@@ -7836,14 +8618,18 @@
       <c r="F165" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G165" s="6">
+      <c r="G165" s="5">
         <v>88050</v>
       </c>
       <c r="H165" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.0794520547945203</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
         <v>103</v>
       </c>
@@ -7862,14 +8648,18 @@
       <c r="F166" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G166" s="6">
+      <c r="G166" s="5">
         <v>100420</v>
       </c>
       <c r="H166" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I166" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1260273972602739</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
         <v>54</v>
       </c>
@@ -7888,14 +8678,18 @@
       <c r="F167" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G167" s="6">
+      <c r="G167" s="5">
         <v>114180</v>
       </c>
       <c r="H167" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I167" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.67671232876712328</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
         <v>86</v>
       </c>
@@ -7914,14 +8708,18 @@
       <c r="F168" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G168" s="6">
+      <c r="G168" s="5">
         <v>33920</v>
       </c>
       <c r="H168" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I168" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.1479452054794521</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
         <v>69</v>
       </c>
@@ -7940,14 +8738,18 @@
       <c r="F169" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G169" s="6">
+      <c r="G169" s="5">
         <v>106460</v>
       </c>
       <c r="H169" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I169" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
         <v>57</v>
       </c>
@@ -7966,14 +8768,18 @@
       <c r="F170" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G170" s="6">
+      <c r="G170" s="5">
         <v>40400</v>
       </c>
       <c r="H170" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0136986301369864</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
         <v>68</v>
       </c>
@@ -7992,14 +8798,18 @@
       <c r="F171" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G171" s="6">
+      <c r="G171" s="5">
         <v>91650</v>
       </c>
       <c r="H171" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I171" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.3589041095890413</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
         <v>99</v>
       </c>
@@ -8018,14 +8828,18 @@
       <c r="F172" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G172" s="6">
+      <c r="G172" s="5">
         <v>36040</v>
       </c>
       <c r="H172" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I172" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3068493150684932</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
         <v>101</v>
       </c>
@@ -8044,14 +8858,18 @@
       <c r="F173" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G173" s="6">
+      <c r="G173" s="5">
         <v>104410</v>
       </c>
       <c r="H173" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9616438356164383</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
         <v>85</v>
       </c>
@@ -8070,14 +8888,18 @@
       <c r="F174" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G174" s="6">
+      <c r="G174" s="5">
         <v>96800</v>
       </c>
       <c r="H174" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I174" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3452054794520547</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="6" t="s">
         <v>28</v>
       </c>
@@ -8096,14 +8918,18 @@
       <c r="F175" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G175" s="6">
+      <c r="G175" s="5">
         <v>85000</v>
       </c>
       <c r="H175" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I175" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.747945205479452</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>80</v>
       </c>
@@ -8122,14 +8948,18 @@
       <c r="F176" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G176" s="6">
+      <c r="G176" s="5">
         <v>43510</v>
       </c>
       <c r="H176" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>0.75890410958904109</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
         <v>79</v>
       </c>
@@ -8148,14 +8978,18 @@
       <c r="F177" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G177" s="6">
+      <c r="G177" s="5">
         <v>59430</v>
       </c>
       <c r="H177" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.3397260273972602</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>93</v>
       </c>
@@ -8174,14 +9008,18 @@
       <c r="F178" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G178" s="6">
+      <c r="G178" s="5">
         <v>65360</v>
       </c>
       <c r="H178" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.8219178082191783</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>66</v>
       </c>
@@ -8200,14 +9038,18 @@
       <c r="F179" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G179" s="6">
+      <c r="G179" s="5">
         <v>41570</v>
       </c>
       <c r="H179" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I179" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.3315068493150686</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>95</v>
       </c>
@@ -8226,14 +9068,18 @@
       <c r="F180" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G180" s="6">
+      <c r="G180" s="5">
         <v>75280</v>
       </c>
       <c r="H180" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>2.1506849315068495</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>18</v>
       </c>
@@ -8252,14 +9098,18 @@
       <c r="F181" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G181" s="6">
+      <c r="G181" s="5">
         <v>74550</v>
       </c>
       <c r="H181" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I181" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.9506849315068493</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>45</v>
       </c>
@@ -8278,14 +9128,18 @@
       <c r="F182" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G182" s="6">
+      <c r="G182" s="5">
         <v>67950</v>
       </c>
       <c r="H182" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I182" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0849315068493151</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="6" t="s">
         <v>90</v>
       </c>
@@ -8304,14 +9158,18 @@
       <c r="F183" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G183" s="6">
+      <c r="G183" s="5">
         <v>70270</v>
       </c>
       <c r="H183" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.0027397260273974</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
         <v>46</v>
       </c>
@@ -8330,17 +9188,25 @@
       <c r="F184" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G184" s="6">
+      <c r="G184" s="5">
         <v>53540</v>
       </c>
       <c r="H184" s="6" t="s">
         <v>207</v>
       </c>
+      <c r="I184" s="9">
+        <f ca="1">(TODAY()-Staff[[#This Row],[Date Joined]])/365</f>
+        <v>1.8794520547945206</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A184">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8349,7 +9215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
male vs female comparison with pivots
</commit_message>
<xml_diff>
--- a/blank-data-file.xlsx
+++ b/blank-data-file.xlsx
@@ -9,22 +9,50 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="India Staff" sheetId="2" r:id="rId2"/>
-    <sheet name="All Staff" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
+    <sheet name="Male vs Female" sheetId="5" r:id="rId4"/>
+    <sheet name="All Staff" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$C$5:$I$105</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'India Staff'!$B$2:$H$114</definedName>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">'All Staff'!$A$1:$H$184</definedName>
+    <definedName name="_xlcn.WorksheetConnection_blankdatafile.xlsxStaff1" hidden="1">Staff[]</definedName>
+    <definedName name="ExternalData_1" localSheetId="4" hidden="1">'All Staff'!$A$1:$H$184</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">Sheet3!$A$3:$I$88</definedName>
+    <definedName name="Slicer_Country">#N/A</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="111" r:id="rId6"/>
+  </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
+      <x14:pivotCaches>
+        <pivotCache cacheId="48" r:id="rId7"/>
+      </x14:pivotCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId8"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="Staff" name="Staff" connection="WorksheetConnection_blank-data-file.xlsx!Staff"/>
+        </x15:modelTables>
+      </x15:dataModel>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,20 +69,46 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - India Staff" description="Connection to the 'India Staff' query in the workbook." type="5" refreshedVersion="0" background="1">
+  <connection id="1" keepAlive="1" name="ModelConnection_ExternalData_1" description="Data Model" type="5" refreshedVersion="6" minRefreshableVersion="5" saveData="1">
+    <dbPr connection="Data Model Connection" command="DRILLTHROUGH MAXROWS 1000 SELECT FROM [Model] WHERE ([Measures].[Average of Age],[Staff].[Gender].&amp;[Female])" commandType="4"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" keepAlive="1" name="Query - India Staff" description="Connection to the 'India Staff' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;India Staff&quot;" command="SELECT * FROM [India Staff]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Query - nz_staff" description="Connection to the 'nz_staff' query in the workbook." type="5" refreshedVersion="0" background="1">
+  <connection id="3" keepAlive="1" name="Query - nz_staff" description="Connection to the 'nz_staff' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=nz_staff" command="SELECT * FROM [nz_staff]"/>
   </connection>
-  <connection id="3" keepAlive="1" name="Query - Staff" description="Connection to the 'Staff' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" keepAlive="1" name="Query - Staff" description="Connection to the 'Staff' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Staff;Extended Properties=&quot;&quot;" command="SELECT * FROM [Staff]"/>
+  </connection>
+  <connection id="5" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="6" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="6" name="WorksheetConnection_blank-data-file.xlsx!Staff" type="102" refreshedVersion="6" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Staff" autoDelete="1">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_blankdatafile.xlsxStaff1"/>
+        </x15:connection>
+      </ext>
+    </extLst>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="240">
   <si>
     <t>Name</t>
   </si>
@@ -726,16 +780,66 @@
   </si>
   <si>
     <t>1.Find salary of a person using VLOOKUP</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Count of Name</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Average of Age</t>
+  </si>
+  <si>
+    <t>Average of Tenure</t>
+  </si>
+  <si>
+    <t>Staff[Name]</t>
+  </si>
+  <si>
+    <t>Staff[Gender]</t>
+  </si>
+  <si>
+    <t>Staff[Age]</t>
+  </si>
+  <si>
+    <t>Staff[Rating]</t>
+  </si>
+  <si>
+    <t>Staff[Date Joined]</t>
+  </si>
+  <si>
+    <t>Staff[Department]</t>
+  </si>
+  <si>
+    <t>Staff[Salary]</t>
+  </si>
+  <si>
+    <t>Staff[Country]</t>
+  </si>
+  <si>
+    <t>Staff[Tenure]</t>
+  </si>
+  <si>
+    <t>Data returned for Average of Age, Female (First 1000 rows).</t>
+  </si>
+  <si>
+    <t>Average of Salary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -805,7 +909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -822,15 +926,177 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="302">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -850,6 +1116,714 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-409]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -900,8 +1874,550 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Country"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Country"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5686425" y="1266825"/>
+              <a:ext cx="1466850" cy="914400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-IN" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="DELL" refreshedDate="45097.775043865739" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="5"/>
+  <cacheFields count="6">
+    <cacheField name="[Staff].[Gender].[Gender]" caption="Gender" numFmtId="0" hierarchy="1" level="1">
+      <sharedItems count="2">
+        <s v="Female"/>
+        <s v="Male"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Measures].[Count of Name]" caption="Count of Name" numFmtId="0" hierarchy="11" level="32767"/>
+    <cacheField name="[Measures].[Average of Age]" caption="Average of Age" numFmtId="0" hierarchy="13" level="32767"/>
+    <cacheField name="[Measures].[Average of Tenure]" caption="Average of Tenure" numFmtId="0" hierarchy="15" level="32767"/>
+    <cacheField name="[Measures].[Average of Salary]" caption="Average of Salary" numFmtId="0" hierarchy="17" level="32767"/>
+    <cacheField name="[Staff].[Country].[Country]" caption="Country" numFmtId="0" hierarchy="7" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsString="0"/>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="18">
+    <cacheHierarchy uniqueName="[Staff].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Staff].[Name].[All]" allUniqueName="[Staff].[Name].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[Staff].[Gender].[All]" allUniqueName="[Staff].[Gender].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Staff].[Age]" caption="Age" attribute="1" defaultMemberUniqueName="[Staff].[Age].[All]" allUniqueName="[Staff].[Age].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Rating]" caption="Rating" attribute="1" defaultMemberUniqueName="[Staff].[Rating].[All]" allUniqueName="[Staff].[Rating].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Date Joined]" caption="Date Joined" attribute="1" time="1" defaultMemberUniqueName="[Staff].[Date Joined].[All]" allUniqueName="[Staff].[Date Joined].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="7" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Department]" caption="Department" attribute="1" defaultMemberUniqueName="[Staff].[Department].[All]" allUniqueName="[Staff].[Department].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Salary]" caption="Salary" attribute="1" defaultMemberUniqueName="[Staff].[Salary].[All]" allUniqueName="[Staff].[Salary].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Country]" caption="Country" attribute="1" defaultMemberUniqueName="[Staff].[Country].[All]" allUniqueName="[Staff].[Country].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="5"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Staff].[Tenure]" caption="Tenure" attribute="1" defaultMemberUniqueName="[Staff].[Tenure].[All]" allUniqueName="[Staff].[Tenure].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count Staff]" caption="__XL_Count Staff" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Count of Name]" caption="Count of Name" measure="1" displayFolder="" measureGroup="Staff" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Age]" caption="Sum of Age" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Age]" caption="Average of Age" measure="1" displayFolder="" measureGroup="Staff" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Tenure]" caption="Sum of Tenure" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="8"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Tenure]" caption="Average of Tenure" measure="1" displayFolder="" measureGroup="Staff" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="3"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="8"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Salary]" caption="Sum of Salary" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="6"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Salary]" caption="Average of Salary" measure="1" displayFolder="" measureGroup="Staff" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="4"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="6"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Staff" uniqueName="[Staff]" caption="Staff"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Staff" caption="Staff"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="DELL" refreshedDate="45097.770763078704" backgroundQuery="1" createdVersion="3" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="5">
+    <extLst>
+      <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
+        <x14:sourceConnection name="ThisWorkbookDataModel"/>
+      </ext>
+    </extLst>
+  </cacheSource>
+  <cacheFields count="0"/>
+  <cacheHierarchies count="18">
+    <cacheHierarchy uniqueName="[Staff].[Name]" caption="Name" attribute="1" defaultMemberUniqueName="[Staff].[Name].[All]" allUniqueName="[Staff].[Name].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Gender]" caption="Gender" attribute="1" defaultMemberUniqueName="[Staff].[Gender].[All]" allUniqueName="[Staff].[Gender].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Age]" caption="Age" attribute="1" defaultMemberUniqueName="[Staff].[Age].[All]" allUniqueName="[Staff].[Age].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Rating]" caption="Rating" attribute="1" defaultMemberUniqueName="[Staff].[Rating].[All]" allUniqueName="[Staff].[Rating].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Date Joined]" caption="Date Joined" attribute="1" time="1" defaultMemberUniqueName="[Staff].[Date Joined].[All]" allUniqueName="[Staff].[Date Joined].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="7" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Department]" caption="Department" attribute="1" defaultMemberUniqueName="[Staff].[Department].[All]" allUniqueName="[Staff].[Department].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Salary]" caption="Salary" attribute="1" defaultMemberUniqueName="[Staff].[Salary].[All]" allUniqueName="[Staff].[Salary].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Country]" caption="Country" attribute="1" defaultMemberUniqueName="[Staff].[Country].[All]" allUniqueName="[Staff].[Country].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Staff].[Tenure]" caption="Tenure" attribute="1" defaultMemberUniqueName="[Staff].[Tenure].[All]" allUniqueName="[Staff].[Tenure].[All]" dimensionUniqueName="[Staff]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count Staff]" caption="__XL_Count Staff" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Count of Name]" caption="Count of Name" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Age]" caption="Sum of Age" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Age]" caption="Average of Age" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Tenure]" caption="Sum of Tenure" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="8"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Tenure]" caption="Average of Tenure" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="8"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Salary]" caption="Sum of Salary" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="6"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Average of Salary]" caption="Average of Salary" measure="1" displayFolder="" measureGroup="Staff" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="6"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition slicerData="1" pivotCacheId="1" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="111" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D7:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="3">
+        <item s="1" x="0"/>
+        <item s="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="Count of Name" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Average of Age" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Salary" fld="4" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Average of Tenure" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="13">
+    <format dxfId="265">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="266">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="267">
+      <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="268">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="269">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="2"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="270">
+      <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="271">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="272">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="273">
+      <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="219">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="218">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="107">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="106">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1">
+            <x v="3"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotHierarchies count="18">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy multipleItemSelectionAllowed="1" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="-2"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="1"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_blank-data-file.xlsx!Staff">
+        <x15:activeTabTopLevelEntity name="[Staff]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" backgroundRefresh="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh nextId="10">
+    <queryTableFields count="9">
+      <queryTableField id="1" name="Staff[Name]" tableColumnId="1"/>
+      <queryTableField id="2" name="Staff[Gender]" tableColumnId="2"/>
+      <queryTableField id="3" name="Staff[Age]" tableColumnId="3"/>
+      <queryTableField id="4" name="Staff[Rating]" tableColumnId="4"/>
+      <queryTableField id="5" name="Staff[Date Joined]" tableColumnId="5"/>
+      <queryTableField id="6" name="Staff[Department]" tableColumnId="6"/>
+      <queryTableField id="7" name="Staff[Salary]" tableColumnId="7"/>
+      <queryTableField id="8" name="Staff[Country]" tableColumnId="8"/>
+      <queryTableField id="9" name="Staff[Tenure]" tableColumnId="9"/>
+    </queryTableFields>
+  </queryTableRefresh>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{883FBD77-0823-4a55-B5E3-86C4891E6966}">
+      <x15:queryTable drillThrough="1"/>
+    </ext>
+  </extLst>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="12" unboundColumnsRight="1">
     <queryTableFields count="9">
       <queryTableField id="1" name="Name" tableColumnId="25"/>
@@ -918,6 +2434,38 @@
 </queryTable>
 </file>
 
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Country" sourceName="[Staff].[Country]">
+  <pivotTables>
+    <pivotTable tabId="5" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <olap pivotCacheId="1">
+      <levels count="2">
+        <level uniqueName="[Staff].[Country].[(All)]" sourceCaption="(All)" count="0"/>
+        <level uniqueName="[Staff].[Country].[Country]" sourceCaption="Country" count="2">
+          <ranges>
+            <range startItem="0">
+              <i n="[Staff].[Country].&amp;[IND]" c="IND"/>
+              <i n="[Staff].[Country].&amp;[NZ]" c="NZ"/>
+            </range>
+          </ranges>
+        </level>
+      </levels>
+      <selections count="1">
+        <selection n="[Staff].[Country].[All]"/>
+      </selections>
+    </olap>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Country" cache="Slicer_Country" caption="Country" level="1" rowHeight="241300"/>
+</slicers>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="nz_staff" displayName="nz_staff" ref="C5:I106" totalsRowCount="1">
   <autoFilter ref="C5:I105"/>
@@ -927,7 +2475,7 @@
     <tableColumn id="3" name="Department"/>
     <tableColumn id="4" name="Age" totalsRowFunction="average"/>
     <tableColumn id="5" name="Date Joined"/>
-    <tableColumn id="6" name="Salary" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="6" name="Salary" totalsRowFunction="average" dataDxfId="301" totalsRowDxfId="300"/>
     <tableColumn id="7" name="Rating" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -942,7 +2490,7 @@
     <tableColumn id="2" name="Gender"/>
     <tableColumn id="3" name="Age"/>
     <tableColumn id="4" name="Rating"/>
-    <tableColumn id="5" name="Date Joined" dataDxfId="11"/>
+    <tableColumn id="5" name="Date Joined" dataDxfId="299"/>
     <tableColumn id="6" name="Department"/>
     <tableColumn id="7" name="Salary"/>
   </tableColumns>
@@ -951,18 +2499,36 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_ExternalData_1" displayName="Table_ExternalData_1" ref="A3:I88" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A3:I88"/>
+  <tableColumns count="9">
+    <tableColumn id="1" uniqueName="1" name="Staff[Name]" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="Staff[Gender]" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="Staff[Age]" queryTableFieldId="3"/>
+    <tableColumn id="4" uniqueName="4" name="Staff[Rating]" queryTableFieldId="4"/>
+    <tableColumn id="5" uniqueName="5" name="Staff[Date Joined]" queryTableFieldId="5" dataDxfId="289"/>
+    <tableColumn id="6" uniqueName="6" name="Staff[Department]" queryTableFieldId="6"/>
+    <tableColumn id="7" uniqueName="7" name="Staff[Salary]" queryTableFieldId="7"/>
+    <tableColumn id="8" uniqueName="8" name="Staff[Country]" queryTableFieldId="8"/>
+    <tableColumn id="9" uniqueName="9" name="Staff[Tenure]" queryTableFieldId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Staff" displayName="Staff" ref="A1:I184" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I184"/>
   <tableColumns count="9">
-    <tableColumn id="25" uniqueName="25" name="Name" queryTableFieldId="1" dataDxfId="10"/>
-    <tableColumn id="26" uniqueName="26" name="Gender" queryTableFieldId="2" dataDxfId="9"/>
-    <tableColumn id="27" uniqueName="27" name="Age" queryTableFieldId="3" dataDxfId="8"/>
-    <tableColumn id="28" uniqueName="28" name="Rating" queryTableFieldId="4" dataDxfId="7"/>
-    <tableColumn id="29" uniqueName="29" name="Date Joined" queryTableFieldId="5" dataDxfId="6"/>
-    <tableColumn id="30" uniqueName="30" name="Department" queryTableFieldId="6" dataDxfId="5"/>
-    <tableColumn id="31" uniqueName="31" name="Salary" queryTableFieldId="7" dataDxfId="4"/>
-    <tableColumn id="32" uniqueName="32" name="Country" queryTableFieldId="8" dataDxfId="3"/>
-    <tableColumn id="1" uniqueName="1" name="Tenure" queryTableFieldId="10" dataDxfId="2">
+    <tableColumn id="25" uniqueName="25" name="Name" queryTableFieldId="1" dataDxfId="298"/>
+    <tableColumn id="26" uniqueName="26" name="Gender" queryTableFieldId="2" dataDxfId="297"/>
+    <tableColumn id="27" uniqueName="27" name="Age" queryTableFieldId="3" dataDxfId="296"/>
+    <tableColumn id="28" uniqueName="28" name="Rating" queryTableFieldId="4" dataDxfId="295"/>
+    <tableColumn id="29" uniqueName="29" name="Date Joined" queryTableFieldId="5" dataDxfId="294"/>
+    <tableColumn id="30" uniqueName="30" name="Department" queryTableFieldId="6" dataDxfId="293"/>
+    <tableColumn id="31" uniqueName="31" name="Salary" queryTableFieldId="7" dataDxfId="292"/>
+    <tableColumn id="32" uniqueName="32" name="Country" queryTableFieldId="8" dataDxfId="291"/>
+    <tableColumn id="1" uniqueName="1" name="Tenure" queryTableFieldId="10" dataDxfId="290">
       <calculatedColumnFormula>(TODAY()-Staff[[#This Row],[Date Joined]])/365</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3619,7 +5185,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:C105">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6236,13 +7802,2633 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I88"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H3" t="s">
+        <v>236</v>
+      </c>
+      <c r="I3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7">
+        <v>44312</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>75280</v>
+      </c>
+      <c r="H4" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4">
+        <v>2.1506849315068495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7">
+        <v>44611</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>41570</v>
+      </c>
+      <c r="H5" t="s">
+        <v>207</v>
+      </c>
+      <c r="I5">
+        <v>1.3315068493150686</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7">
+        <v>44067</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>65360</v>
+      </c>
+      <c r="H6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6">
+        <v>2.8219178082191783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7">
+        <v>44459</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>85000</v>
+      </c>
+      <c r="H7" t="s">
+        <v>207</v>
+      </c>
+      <c r="I7">
+        <v>1.747945205479452</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7">
+        <v>44381</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>104410</v>
+      </c>
+      <c r="H8" t="s">
+        <v>207</v>
+      </c>
+      <c r="I8">
+        <v>1.9616438356164383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7">
+        <v>44678</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>33920</v>
+      </c>
+      <c r="H9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9">
+        <v>1.1479452054794521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="7">
+        <v>44850</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>114180</v>
+      </c>
+      <c r="H10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I10">
+        <v>0.67671232876712328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="7">
+        <v>44649</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>104120</v>
+      </c>
+      <c r="H11" t="s">
+        <v>207</v>
+      </c>
+      <c r="I11">
+        <v>1.2273972602739727</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="7">
+        <v>44317</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12">
+        <v>65920</v>
+      </c>
+      <c r="H12" t="s">
+        <v>207</v>
+      </c>
+      <c r="I12">
+        <v>2.1369863013698631</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="7">
+        <v>44205</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>92700</v>
+      </c>
+      <c r="H13" t="s">
+        <v>207</v>
+      </c>
+      <c r="I13">
+        <v>2.4438356164383563</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="7">
+        <v>44329</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14">
+        <v>56870</v>
+      </c>
+      <c r="H14" t="s">
+        <v>207</v>
+      </c>
+      <c r="I14">
+        <v>2.1041095890410957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="7">
+        <v>44486</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>104770</v>
+      </c>
+      <c r="H15" t="s">
+        <v>207</v>
+      </c>
+      <c r="I15">
+        <v>1.6739726027397259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="7">
+        <v>45045</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>114870</v>
+      </c>
+      <c r="H16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I16">
+        <v>0.14246575342465753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="7">
+        <v>44450</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>76900</v>
+      </c>
+      <c r="H17" t="s">
+        <v>207</v>
+      </c>
+      <c r="I17">
+        <v>1.7726027397260273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="7">
+        <v>44451</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18">
+        <v>118100</v>
+      </c>
+      <c r="H18" t="s">
+        <v>207</v>
+      </c>
+      <c r="I18">
+        <v>1.7698630136986302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="7">
+        <v>44377</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19">
+        <v>109160</v>
+      </c>
+      <c r="H19" t="s">
+        <v>207</v>
+      </c>
+      <c r="I19">
+        <v>1.9726027397260273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="7">
+        <v>44085</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>114890</v>
+      </c>
+      <c r="H20" t="s">
+        <v>207</v>
+      </c>
+      <c r="I20">
+        <v>2.7726027397260276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="7">
+        <v>44400</v>
+      </c>
+      <c r="F21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21">
+        <v>45510</v>
+      </c>
+      <c r="H21" t="s">
+        <v>207</v>
+      </c>
+      <c r="I21">
+        <v>1.9095890410958904</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="7">
+        <v>44694</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <v>80700</v>
+      </c>
+      <c r="H22" t="s">
+        <v>207</v>
+      </c>
+      <c r="I22">
+        <v>1.1041095890410959</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>44537</v>
+      </c>
+      <c r="F23" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23">
+        <v>68900</v>
+      </c>
+      <c r="H23" t="s">
+        <v>207</v>
+      </c>
+      <c r="I23">
+        <v>1.5342465753424657</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>34</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="7">
+        <v>44445</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24">
+        <v>92450</v>
+      </c>
+      <c r="H24" t="s">
+        <v>207</v>
+      </c>
+      <c r="I24">
+        <v>1.7863013698630137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="7">
+        <v>44686</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <v>83750</v>
+      </c>
+      <c r="H25" t="s">
+        <v>207</v>
+      </c>
+      <c r="I25">
+        <v>1.1260273972602739</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="7">
+        <v>44809</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26">
+        <v>86570</v>
+      </c>
+      <c r="H26" t="s">
+        <v>207</v>
+      </c>
+      <c r="I26">
+        <v>0.78904109589041094</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="7">
+        <v>44529</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>78390</v>
+      </c>
+      <c r="H27" t="s">
+        <v>207</v>
+      </c>
+      <c r="I27">
+        <v>1.5561643835616439</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="7">
+        <v>44190</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28">
+        <v>96140</v>
+      </c>
+      <c r="H28" t="s">
+        <v>207</v>
+      </c>
+      <c r="I28">
+        <v>2.484931506849315</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="7">
+        <v>44630</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29">
+        <v>99970</v>
+      </c>
+      <c r="H29" t="s">
+        <v>207</v>
+      </c>
+      <c r="I29">
+        <v>1.2794520547945205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="7">
+        <v>44721</v>
+      </c>
+      <c r="F30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30">
+        <v>49630</v>
+      </c>
+      <c r="H30" t="s">
+        <v>207</v>
+      </c>
+      <c r="I30">
+        <v>1.0301369863013699</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>36</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="7">
+        <v>44494</v>
+      </c>
+      <c r="F31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31">
+        <v>78540</v>
+      </c>
+      <c r="H31" t="s">
+        <v>207</v>
+      </c>
+      <c r="I31">
+        <v>1.6520547945205479</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="7">
+        <v>44374</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32">
+        <v>75480</v>
+      </c>
+      <c r="H32" t="s">
+        <v>207</v>
+      </c>
+      <c r="I32">
+        <v>1.9808219178082191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="7">
+        <v>44612</v>
+      </c>
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+      <c r="G33">
+        <v>60130</v>
+      </c>
+      <c r="H33" t="s">
+        <v>207</v>
+      </c>
+      <c r="I33">
+        <v>1.3287671232876712</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="7">
+        <v>44185</v>
+      </c>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34">
+        <v>75970</v>
+      </c>
+      <c r="H34" t="s">
+        <v>207</v>
+      </c>
+      <c r="I34">
+        <v>2.4986301369863013</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>29</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="7">
+        <v>44023</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>34980</v>
+      </c>
+      <c r="H35" t="s">
+        <v>207</v>
+      </c>
+      <c r="I35">
+        <v>2.9424657534246577</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>40</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="7">
+        <v>44337</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <v>87620</v>
+      </c>
+      <c r="H36" t="s">
+        <v>207</v>
+      </c>
+      <c r="I36">
+        <v>2.0821917808219177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="7">
+        <v>44779</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <v>75000</v>
+      </c>
+      <c r="H37" t="s">
+        <v>207</v>
+      </c>
+      <c r="I37">
+        <v>0.87123287671232874</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>31</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="7">
+        <v>44663</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38">
+        <v>58100</v>
+      </c>
+      <c r="H38" t="s">
+        <v>207</v>
+      </c>
+      <c r="I38">
+        <v>1.189041095890411</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="7">
+        <v>44389</v>
+      </c>
+      <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39">
+        <v>67910</v>
+      </c>
+      <c r="H39" t="s">
+        <v>207</v>
+      </c>
+      <c r="I39">
+        <v>1.9397260273972603</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>34</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="7">
+        <v>44653</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40">
+        <v>58940</v>
+      </c>
+      <c r="H40" t="s">
+        <v>207</v>
+      </c>
+      <c r="I40">
+        <v>1.2164383561643837</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>31</v>
+      </c>
+      <c r="D41" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="7">
+        <v>44145</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41">
+        <v>41980</v>
+      </c>
+      <c r="H41" t="s">
+        <v>207</v>
+      </c>
+      <c r="I41">
+        <v>2.6082191780821917</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>32</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="7">
+        <v>44354</v>
+      </c>
+      <c r="F42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42">
+        <v>43840</v>
+      </c>
+      <c r="H42" t="s">
+        <v>207</v>
+      </c>
+      <c r="I42">
+        <v>2.0356164383561643</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="7">
+        <v>44122</v>
+      </c>
+      <c r="F43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43">
+        <v>119110</v>
+      </c>
+      <c r="H43" t="s">
+        <v>207</v>
+      </c>
+      <c r="I43">
+        <v>2.6712328767123288</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>24</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="7">
+        <v>44148</v>
+      </c>
+      <c r="F44" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44">
+        <v>62780</v>
+      </c>
+      <c r="H44" t="s">
+        <v>207</v>
+      </c>
+      <c r="I44">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>30</v>
+      </c>
+      <c r="D45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="7">
+        <v>44861</v>
+      </c>
+      <c r="F45" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>112570</v>
+      </c>
+      <c r="H45" t="s">
+        <v>207</v>
+      </c>
+      <c r="I45">
+        <v>0.64657534246575343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="7">
+        <v>44357</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46">
+        <v>53240</v>
+      </c>
+      <c r="H46" t="s">
+        <v>207</v>
+      </c>
+      <c r="I46">
+        <v>2.0273972602739727</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="7">
+        <v>44129</v>
+      </c>
+      <c r="F47" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47">
+        <v>96140</v>
+      </c>
+      <c r="H47" t="s">
+        <v>205</v>
+      </c>
+      <c r="I47">
+        <v>2.6520547945205482</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>36</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="7">
+        <v>44433</v>
+      </c>
+      <c r="F48" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48">
+        <v>78540</v>
+      </c>
+      <c r="H48" t="s">
+        <v>205</v>
+      </c>
+      <c r="I48">
+        <v>1.8191780821917809</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="7">
+        <v>44313</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49">
+        <v>75480</v>
+      </c>
+      <c r="H49" t="s">
+        <v>205</v>
+      </c>
+      <c r="I49">
+        <v>2.1479452054794521</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>24</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="7">
+        <v>44087</v>
+      </c>
+      <c r="F50" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50">
+        <v>62780</v>
+      </c>
+      <c r="H50" t="s">
+        <v>205</v>
+      </c>
+      <c r="I50">
+        <v>2.7671232876712328</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>29</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="7">
+        <v>43962</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51">
+        <v>34980</v>
+      </c>
+      <c r="H51" t="s">
+        <v>205</v>
+      </c>
+      <c r="I51">
+        <v>3.1095890410958904</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>189</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>28</v>
+      </c>
+      <c r="D52" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="7">
+        <v>44590</v>
+      </c>
+      <c r="F52" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52">
+        <v>104120</v>
+      </c>
+      <c r="H52" t="s">
+        <v>205</v>
+      </c>
+      <c r="I52">
+        <v>1.3890410958904109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <v>30</v>
+      </c>
+      <c r="D53" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="7">
+        <v>44789</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53">
+        <v>114180</v>
+      </c>
+      <c r="H53" t="s">
+        <v>205</v>
+      </c>
+      <c r="I53">
+        <v>0.84383561643835614</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>36</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="7">
+        <v>44468</v>
+      </c>
+      <c r="F54" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54">
+        <v>78390</v>
+      </c>
+      <c r="H54" t="s">
+        <v>205</v>
+      </c>
+      <c r="I54">
+        <v>1.7232876712328766</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>148</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>37</v>
+      </c>
+      <c r="D55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="7">
+        <v>44389</v>
+      </c>
+      <c r="F55" t="s">
+        <v>56</v>
+      </c>
+      <c r="G55">
+        <v>118100</v>
+      </c>
+      <c r="H55" t="s">
+        <v>205</v>
+      </c>
+      <c r="I55">
+        <v>1.9397260273972603</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>132</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <v>34</v>
+      </c>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="7">
+        <v>44550</v>
+      </c>
+      <c r="F56" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56">
+        <v>60130</v>
+      </c>
+      <c r="H56" t="s">
+        <v>205</v>
+      </c>
+      <c r="I56">
+        <v>1.4986301369863013</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>30</v>
+      </c>
+      <c r="D57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="7">
+        <v>44328</v>
+      </c>
+      <c r="F57" t="s">
+        <v>21</v>
+      </c>
+      <c r="G57">
+        <v>67910</v>
+      </c>
+      <c r="H57" t="s">
+        <v>205</v>
+      </c>
+      <c r="I57">
+        <v>2.106849315068493</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>33</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="7">
+        <v>44747</v>
+      </c>
+      <c r="F58" t="s">
+        <v>21</v>
+      </c>
+      <c r="G58">
+        <v>86570</v>
+      </c>
+      <c r="H58" t="s">
+        <v>205</v>
+      </c>
+      <c r="I58">
+        <v>0.95890410958904104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>31</v>
+      </c>
+      <c r="D59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="7">
+        <v>44084</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59">
+        <v>41980</v>
+      </c>
+      <c r="H59" t="s">
+        <v>205</v>
+      </c>
+      <c r="I59">
+        <v>2.7753424657534245</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="7">
+        <v>44316</v>
+      </c>
+      <c r="F60" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60">
+        <v>109160</v>
+      </c>
+      <c r="H60" t="s">
+        <v>205</v>
+      </c>
+      <c r="I60">
+        <v>2.1397260273972605</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>20</v>
+      </c>
+      <c r="D61" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="7">
+        <v>44476</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61">
+        <v>68900</v>
+      </c>
+      <c r="H61" t="s">
+        <v>205</v>
+      </c>
+      <c r="I61">
+        <v>1.7013698630136986</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>40</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="7">
+        <v>44276</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62">
+        <v>87620</v>
+      </c>
+      <c r="H62" t="s">
+        <v>205</v>
+      </c>
+      <c r="I62">
+        <v>2.2493150684931509</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>185</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>27</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63" s="7">
+        <v>44625</v>
+      </c>
+      <c r="F63" t="s">
+        <v>12</v>
+      </c>
+      <c r="G63">
+        <v>83750</v>
+      </c>
+      <c r="H63" t="s">
+        <v>205</v>
+      </c>
+      <c r="I63">
+        <v>1.2931506849315069</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>195</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>34</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="7">
+        <v>44383</v>
+      </c>
+      <c r="F64" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64">
+        <v>92450</v>
+      </c>
+      <c r="H64" t="s">
+        <v>205</v>
+      </c>
+      <c r="I64">
+        <v>1.9561643835616438</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>33</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" s="7">
+        <v>44006</v>
+      </c>
+      <c r="F65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65">
+        <v>65360</v>
+      </c>
+      <c r="H65" t="s">
+        <v>205</v>
+      </c>
+      <c r="I65">
+        <v>2.989041095890411</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>28</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="7">
+        <v>44124</v>
+      </c>
+      <c r="F66" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66">
+        <v>75970</v>
+      </c>
+      <c r="H66" t="s">
+        <v>205</v>
+      </c>
+      <c r="I66">
+        <v>2.6657534246575341</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>28</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67" s="7">
+        <v>44425</v>
+      </c>
+      <c r="F67" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67">
+        <v>104770</v>
+      </c>
+      <c r="H67" t="s">
+        <v>205</v>
+      </c>
+      <c r="I67">
+        <v>1.8410958904109589</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68">
+        <v>34</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" s="7">
+        <v>44594</v>
+      </c>
+      <c r="F68" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68">
+        <v>58940</v>
+      </c>
+      <c r="H68" t="s">
+        <v>205</v>
+      </c>
+      <c r="I68">
+        <v>1.3780821917808219</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>188</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69">
+        <v>33</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" s="7">
+        <v>44253</v>
+      </c>
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69">
+        <v>75280</v>
+      </c>
+      <c r="H69" t="s">
+        <v>205</v>
+      </c>
+      <c r="I69">
+        <v>2.3123287671232875</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>179</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>21</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="7">
+        <v>44619</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70">
+        <v>33920</v>
+      </c>
+      <c r="H70" t="s">
+        <v>205</v>
+      </c>
+      <c r="I70">
+        <v>1.3095890410958904</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71">
+        <v>34</v>
+      </c>
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" s="7">
+        <v>44397</v>
+      </c>
+      <c r="F71" t="s">
+        <v>21</v>
+      </c>
+      <c r="G71">
+        <v>85000</v>
+      </c>
+      <c r="H71" t="s">
+        <v>205</v>
+      </c>
+      <c r="I71">
+        <v>1.9178082191780821</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <v>28</v>
+      </c>
+      <c r="D72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="7">
+        <v>44296</v>
+      </c>
+      <c r="F72" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72">
+        <v>53240</v>
+      </c>
+      <c r="H72" t="s">
+        <v>205</v>
+      </c>
+      <c r="I72">
+        <v>2.1945205479452055</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73">
+        <v>36</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="7">
+        <v>44023</v>
+      </c>
+      <c r="F73" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73">
+        <v>114890</v>
+      </c>
+      <c r="H73" t="s">
+        <v>205</v>
+      </c>
+      <c r="I73">
+        <v>2.9424657534246577</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74">
+        <v>27</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="7">
+        <v>44061</v>
+      </c>
+      <c r="F74" t="s">
+        <v>56</v>
+      </c>
+      <c r="G74">
+        <v>119110</v>
+      </c>
+      <c r="H74" t="s">
+        <v>205</v>
+      </c>
+      <c r="I74">
+        <v>2.8383561643835615</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>133</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75">
+        <v>25</v>
+      </c>
+      <c r="D75" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="7">
+        <v>44633</v>
+      </c>
+      <c r="F75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G75">
+        <v>80700</v>
+      </c>
+      <c r="H75" t="s">
+        <v>205</v>
+      </c>
+      <c r="I75">
+        <v>1.2712328767123289</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>200</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76">
+        <v>28</v>
+      </c>
+      <c r="D76" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" s="7">
+        <v>44571</v>
+      </c>
+      <c r="F76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76">
+        <v>99970</v>
+      </c>
+      <c r="H76" t="s">
+        <v>205</v>
+      </c>
+      <c r="I76">
+        <v>1.441095890410959</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>126</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <v>21</v>
+      </c>
+      <c r="D77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="7">
+        <v>44256</v>
+      </c>
+      <c r="F77" t="s">
+        <v>21</v>
+      </c>
+      <c r="G77">
+        <v>65920</v>
+      </c>
+      <c r="H77" t="s">
+        <v>205</v>
+      </c>
+      <c r="I77">
+        <v>2.3041095890410959</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>173</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>30</v>
+      </c>
+      <c r="D78" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" s="7">
+        <v>44800</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78">
+        <v>112570</v>
+      </c>
+      <c r="H78" t="s">
+        <v>205</v>
+      </c>
+      <c r="I78">
+        <v>0.81369863013698629</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>32</v>
+      </c>
+      <c r="D79" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79" s="7">
+        <v>44549</v>
+      </c>
+      <c r="F79" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79">
+        <v>41570</v>
+      </c>
+      <c r="H79" t="s">
+        <v>205</v>
+      </c>
+      <c r="I79">
+        <v>1.5013698630136987</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80">
+        <v>44</v>
+      </c>
+      <c r="D80" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80" s="7">
+        <v>44985</v>
+      </c>
+      <c r="F80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80">
+        <v>114870</v>
+      </c>
+      <c r="H80" t="s">
+        <v>205</v>
+      </c>
+      <c r="I80">
+        <v>0.30684931506849317</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>120</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>31</v>
+      </c>
+      <c r="D81" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81" s="7">
+        <v>44604</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81">
+        <v>58100</v>
+      </c>
+      <c r="H81" t="s">
+        <v>205</v>
+      </c>
+      <c r="I81">
+        <v>1.3506849315068492</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>42</v>
+      </c>
+      <c r="D82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="7">
+        <v>44718</v>
+      </c>
+      <c r="F82" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82">
+        <v>75000</v>
+      </c>
+      <c r="H82" t="s">
+        <v>205</v>
+      </c>
+      <c r="I82">
+        <v>1.0383561643835617</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>154</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>22</v>
+      </c>
+      <c r="D83" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="7">
+        <v>44388</v>
+      </c>
+      <c r="F83" t="s">
+        <v>9</v>
+      </c>
+      <c r="G83">
+        <v>76900</v>
+      </c>
+      <c r="H83" t="s">
+        <v>205</v>
+      </c>
+      <c r="I83">
+        <v>1.9424657534246574</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>165</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84">
+        <v>34</v>
+      </c>
+      <c r="D84" t="s">
+        <v>24</v>
+      </c>
+      <c r="E84" s="7">
+        <v>44660</v>
+      </c>
+      <c r="F84" t="s">
+        <v>19</v>
+      </c>
+      <c r="G84">
+        <v>49630</v>
+      </c>
+      <c r="H84" t="s">
+        <v>205</v>
+      </c>
+      <c r="I84">
+        <v>1.1972602739726028</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>169</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85">
+        <v>25</v>
+      </c>
+      <c r="D85" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85" s="7">
+        <v>44144</v>
+      </c>
+      <c r="F85" t="s">
+        <v>19</v>
+      </c>
+      <c r="G85">
+        <v>92700</v>
+      </c>
+      <c r="H85" t="s">
+        <v>205</v>
+      </c>
+      <c r="I85">
+        <v>2.6109589041095891</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>202</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>38</v>
+      </c>
+      <c r="D86" t="s">
+        <v>13</v>
+      </c>
+      <c r="E86" s="7">
+        <v>44268</v>
+      </c>
+      <c r="F86" t="s">
+        <v>19</v>
+      </c>
+      <c r="G86">
+        <v>56870</v>
+      </c>
+      <c r="H86" t="s">
+        <v>205</v>
+      </c>
+      <c r="I86">
+        <v>2.2712328767123289</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>201</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87">
+        <v>32</v>
+      </c>
+      <c r="D87" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="7">
+        <v>44339</v>
+      </c>
+      <c r="F87" t="s">
+        <v>56</v>
+      </c>
+      <c r="G87">
+        <v>45510</v>
+      </c>
+      <c r="H87" t="s">
+        <v>205</v>
+      </c>
+      <c r="I87">
+        <v>2.0767123287671234</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88">
+        <v>32</v>
+      </c>
+      <c r="D88" t="s">
+        <v>13</v>
+      </c>
+      <c r="E88" s="7">
+        <v>44293</v>
+      </c>
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88">
+        <v>43840</v>
+      </c>
+      <c r="H88" t="s">
+        <v>205</v>
+      </c>
+      <c r="I88">
+        <v>2.2027397260273971</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D7:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="E9" s="6">
+        <v>85</v>
+      </c>
+      <c r="F9" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="E10" s="16">
+        <v>31.305882352941175</v>
+      </c>
+      <c r="F10" s="16">
+        <v>29.393258426966291</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="E11" s="17">
+        <v>77976.823529411762</v>
+      </c>
+      <c r="F11" s="17">
+        <v>74915.168539325838</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D12" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="16">
+        <v>1.8180499597099111</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1.8125596429121138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:N184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11880,7 +16066,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A184">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>